<commit_message>
[IMP] Adjust CD Receivable balance sheet summary
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_balance_sheet_summary.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_balance_sheet_summary.xlsx
@@ -9,10 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="Receivable CD Balance Sheet Summary Report" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="brought_forward_detail_report" sheetId="2" state="hidden" r:id="rId3"/>
-    <sheet name="brought_forward_report" sheetId="3" state="hidden" r:id="rId4"/>
-    <sheet name="received_detail_report" sheetId="4" state="hidden" r:id="rId5"/>
-    <sheet name="received_report" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve">Receivable Balance Sheet Summary Report</t>
   </si>
@@ -93,12 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">Outstanding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loan Agreement ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payment Amount (Supplier +, Customer -)</t>
   </si>
 </sst>
 </file>
@@ -107,7 +97,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00_);\(#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="#,###.00"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="5">
@@ -140,7 +130,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,12 +149,6 @@
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF200"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
@@ -200,7 +184,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -217,6 +201,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,7 +229,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -265,7 +253,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -345,122 +333,133 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="41.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="38.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="24.6"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="3" width="28.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="28.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="4" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4"/>
-    </row>
-    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="D3" s="8"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-    </row>
-    <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="B4" s="8"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="D5" s="8"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="D6" s="9"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="B7" s="8"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7"/>
-    </row>
-    <row r="9" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="B8" s="8"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="B9" s="8"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7"/>
-    </row>
-    <row r="11" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="B10" s="8"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="8"/>
-    </row>
-    <row r="12" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="B11" s="9"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="L13" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -471,160 +470,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.08"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>